<commit_message>
Added the correct coupled isotherm featuer to the column model in preparation of expieraments on Borate and HCl optmization
</commit_message>
<xml_diff>
--- a/case3_Borate/_bor_hcl_UBK_530.xlsx
+++ b/case3_Borate/_bor_hcl_UBK_530.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO_Papers\MEng_Code\case3_Borate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1979230255d33e2/Desktop/MEng/MEng_Code/case3_Borate/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D96FF0-7823-4A89-BBF7-F2EA42E08B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -446,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -482,7 +482,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -492,21 +491,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2339,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2385,10 +2378,10 @@
       <c r="F1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I1" s="7" t="s">
@@ -2457,11 +2450,11 @@
       <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2" s="23">
-        <f>E3*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="23">
+      <c r="G2" s="22">
+        <f t="shared" ref="G2:G35" si="1">E3*0.000001</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="22">
         <f>F2*0.000001</f>
         <v>0</v>
       </c>
@@ -2526,21 +2519,21 @@
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="19">
         <v>36</v>
       </c>
-      <c r="E3" s="22">
-        <v>0</v>
-      </c>
-      <c r="F3" s="21">
+      <c r="E3" s="21">
+        <v>0</v>
+      </c>
+      <c r="F3" s="20">
         <v>97.86</v>
       </c>
-      <c r="G3" s="23">
-        <f>E4*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="23">
-        <f t="shared" ref="H3:H35" si="1">F3*0.000001</f>
+      <c r="G3" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="22">
+        <f t="shared" ref="H3:H35" si="2">F3*0.000001</f>
         <v>9.7860000000000002E-5</v>
       </c>
       <c r="M3" s="4"/>
@@ -2560,21 +2553,21 @@
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="19">
         <v>72</v>
       </c>
-      <c r="E4" s="22">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="E4" s="21">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20">
         <v>73.38</v>
       </c>
-      <c r="G4" s="23">
-        <f>E5*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="23">
+      <c r="G4" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="22">
+        <f t="shared" si="2"/>
         <v>7.3379999999999992E-5</v>
       </c>
       <c r="J4" s="7" t="s">
@@ -2598,21 +2591,21 @@
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="19">
         <v>108</v>
       </c>
-      <c r="E5" s="22">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="E5" s="21">
+        <v>0</v>
+      </c>
+      <c r="F5" s="20">
         <v>93.97</v>
       </c>
-      <c r="G5" s="23">
-        <f>E6*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="23">
+      <c r="G5" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="22">
+        <f t="shared" si="2"/>
         <v>9.3969999999999996E-5</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -2637,21 +2630,21 @@
         <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="19">
         <v>144</v>
       </c>
-      <c r="E6" s="22">
-        <v>0</v>
-      </c>
-      <c r="F6" s="21">
+      <c r="E6" s="21">
+        <v>0</v>
+      </c>
+      <c r="F6" s="20">
         <v>13.52</v>
       </c>
-      <c r="G6" s="23">
-        <f>E7*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="23">
+      <c r="G6" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="22">
+        <f t="shared" si="2"/>
         <v>1.3519999999999999E-5</v>
       </c>
     </row>
@@ -2666,21 +2659,21 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <v>180</v>
       </c>
-      <c r="E7" s="22">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="E7" s="21">
+        <v>0</v>
+      </c>
+      <c r="F7" s="20">
         <v>12.93</v>
       </c>
-      <c r="G7" s="23">
-        <f>E8*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="23">
+      <c r="G7" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="22">
+        <f t="shared" si="2"/>
         <v>1.293E-5</v>
       </c>
     </row>
@@ -2695,21 +2688,21 @@
         <f t="shared" si="0"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <v>216</v>
       </c>
-      <c r="E8" s="22">
-        <v>0</v>
-      </c>
-      <c r="F8" s="21">
+      <c r="E8" s="21">
+        <v>0</v>
+      </c>
+      <c r="F8" s="20">
         <v>293.19</v>
       </c>
-      <c r="G8" s="23">
-        <f>E9*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="23">
+      <c r="G8" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="22">
+        <f t="shared" si="2"/>
         <v>2.9318999999999998E-4</v>
       </c>
       <c r="I8" s="2"/>
@@ -2725,21 +2718,21 @@
         <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="19">
         <v>252</v>
       </c>
-      <c r="E9" s="22">
-        <v>0</v>
-      </c>
-      <c r="F9" s="21">
+      <c r="E9" s="21">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20">
         <v>5880.77</v>
       </c>
-      <c r="G9" s="23">
-        <f>E10*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="23">
+      <c r="G9" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="22">
+        <f t="shared" si="2"/>
         <v>5.8807700000000004E-3</v>
       </c>
       <c r="I9" s="2"/>
@@ -2755,20 +2748,20 @@
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="19">
         <v>288</v>
       </c>
-      <c r="E10" s="22">
-        <v>0</v>
-      </c>
-      <c r="F10" s="21">
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="20">
         <v>9372.2999999999993</v>
       </c>
-      <c r="G10" s="23">
-        <f>E11*0.000001</f>
+      <c r="G10" s="22">
+        <f t="shared" si="1"/>
         <v>8.419999999999999E-6</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="22">
         <f>F10*0.000001</f>
         <v>9.3722999999999983E-3</v>
       </c>
@@ -2785,21 +2778,21 @@
         <f t="shared" si="0"/>
         <v>5.3999999999999995</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="19">
         <v>324</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <v>8.42</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="20">
         <v>10097.93</v>
       </c>
-      <c r="G11" s="23">
-        <f>E12*0.000001</f>
+      <c r="G11" s="22">
+        <f t="shared" si="1"/>
         <v>9.7359999999999989E-5</v>
       </c>
-      <c r="H11" s="23">
-        <f t="shared" si="1"/>
+      <c r="H11" s="22">
+        <f t="shared" si="2"/>
         <v>1.009793E-2</v>
       </c>
     </row>
@@ -2814,21 +2807,21 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="19">
         <v>360</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <v>97.36</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <v>10235.74</v>
       </c>
-      <c r="G12" s="23">
-        <f>E13*0.000001</f>
+      <c r="G12" s="22">
+        <f t="shared" si="1"/>
         <v>3.6158999999999996E-4</v>
       </c>
-      <c r="H12" s="23">
-        <f t="shared" si="1"/>
+      <c r="H12" s="22">
+        <f t="shared" si="2"/>
         <v>1.023574E-2</v>
       </c>
       <c r="I12" s="2"/>
@@ -2844,21 +2837,21 @@
         <f t="shared" si="0"/>
         <v>6.6</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="19">
         <v>396</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="21">
         <v>361.59</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="20">
         <v>10486.39</v>
       </c>
-      <c r="G13" s="23">
-        <f>E14*0.000001</f>
+      <c r="G13" s="22">
+        <f t="shared" si="1"/>
         <v>6.9425999999999993E-4</v>
       </c>
-      <c r="H13" s="23">
-        <f t="shared" si="1"/>
+      <c r="H13" s="22">
+        <f t="shared" si="2"/>
         <v>1.0486389999999998E-2</v>
       </c>
       <c r="I13" s="2"/>
@@ -2874,21 +2867,21 @@
         <f t="shared" si="0"/>
         <v>7.1999999999999993</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="19">
         <v>432</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="21">
         <v>694.26</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <v>10332.620000000001</v>
       </c>
-      <c r="G14" s="23">
-        <f>E15*0.000001</f>
+      <c r="G14" s="22">
+        <f t="shared" si="1"/>
         <v>1.1298599999999999E-3</v>
       </c>
-      <c r="H14" s="23">
-        <f t="shared" si="1"/>
+      <c r="H14" s="22">
+        <f t="shared" si="2"/>
         <v>1.0332620000000001E-2</v>
       </c>
       <c r="I14" s="2"/>
@@ -2904,21 +2897,21 @@
         <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="19">
         <v>468</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="21">
         <v>1129.8599999999999</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <v>43.91</v>
       </c>
-      <c r="G15" s="23">
-        <f>E16*0.000001</f>
+      <c r="G15" s="22">
+        <f t="shared" si="1"/>
         <v>1.4159800000000001E-3</v>
       </c>
-      <c r="H15" s="23">
-        <f t="shared" si="1"/>
+      <c r="H15" s="22">
+        <f t="shared" si="2"/>
         <v>4.3909999999999991E-5</v>
       </c>
       <c r="I15" s="2"/>
@@ -2934,21 +2927,21 @@
         <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="19">
         <v>504</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="21">
         <v>1415.98</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>122.91</v>
       </c>
-      <c r="G16" s="23">
-        <f>E17*0.000001</f>
+      <c r="G16" s="22">
+        <f t="shared" si="1"/>
         <v>1.4542799999999999E-3</v>
       </c>
-      <c r="H16" s="23">
-        <f t="shared" si="1"/>
+      <c r="H16" s="22">
+        <f t="shared" si="2"/>
         <v>1.2291E-4</v>
       </c>
       <c r="I16" s="2"/>
@@ -2964,21 +2957,21 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <v>540</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>1454.28</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <v>113.52</v>
       </c>
-      <c r="G17" s="23">
-        <f>E18*0.000001</f>
+      <c r="G17" s="22">
+        <f t="shared" si="1"/>
         <v>1.3279500000000001E-3</v>
       </c>
-      <c r="H17" s="23">
-        <f t="shared" si="1"/>
+      <c r="H17" s="22">
+        <f t="shared" si="2"/>
         <v>1.1352E-4</v>
       </c>
       <c r="I17" s="2"/>
@@ -2994,21 +2987,21 @@
         <f t="shared" si="0"/>
         <v>9.6</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="19">
         <v>576</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="21">
         <v>1327.95</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="20">
         <v>117.21</v>
       </c>
-      <c r="G18" s="23">
-        <f>E19*0.000001</f>
+      <c r="G18" s="22">
+        <f t="shared" si="1"/>
         <v>8.7770999999999997E-4</v>
       </c>
-      <c r="H18" s="23">
-        <f t="shared" si="1"/>
+      <c r="H18" s="22">
+        <f t="shared" si="2"/>
         <v>1.1720999999999998E-4</v>
       </c>
       <c r="I18" s="2"/>
@@ -3024,21 +3017,21 @@
         <f t="shared" si="0"/>
         <v>10.199999999999999</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="19">
         <v>612</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="21">
         <v>877.71</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="20">
         <v>111.15</v>
       </c>
-      <c r="G19" s="23">
-        <f>E20*0.000001</f>
+      <c r="G19" s="22">
+        <f t="shared" si="1"/>
         <v>3.9789999999999997E-4</v>
       </c>
-      <c r="H19" s="23">
-        <f t="shared" si="1"/>
+      <c r="H19" s="22">
+        <f t="shared" si="2"/>
         <v>1.1115E-4</v>
       </c>
       <c r="I19" s="2"/>
@@ -3054,21 +3047,21 @@
         <f t="shared" si="0"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="19">
         <v>648</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="21">
         <v>397.9</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="20">
         <v>3.17</v>
       </c>
-      <c r="G20" s="23">
-        <f>E21*0.000001</f>
+      <c r="G20" s="22">
+        <f t="shared" si="1"/>
         <v>1.1509E-4</v>
       </c>
-      <c r="H20" s="23">
-        <f t="shared" si="1"/>
+      <c r="H20" s="22">
+        <f t="shared" si="2"/>
         <v>3.1699999999999997E-6</v>
       </c>
       <c r="I20" s="2"/>
@@ -3084,21 +3077,21 @@
         <f t="shared" si="0"/>
         <v>11.4</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="19">
         <v>684</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="21">
         <v>115.09</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="20">
         <v>150.94</v>
       </c>
-      <c r="G21" s="23">
-        <f>E22*0.000001</f>
+      <c r="G21" s="22">
+        <f t="shared" si="1"/>
         <v>2.4069999999999998E-5</v>
       </c>
-      <c r="H21" s="23">
-        <f t="shared" si="1"/>
+      <c r="H21" s="22">
+        <f t="shared" si="2"/>
         <v>1.5093999999999999E-4</v>
       </c>
       <c r="I21" s="2"/>
@@ -3114,21 +3107,21 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="19">
         <v>720</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <v>24.07</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="20">
         <v>122.93</v>
       </c>
-      <c r="G22" s="23">
-        <f>E23*0.000001</f>
+      <c r="G22" s="22">
+        <f t="shared" si="1"/>
         <v>6.8099999999999992E-6</v>
       </c>
-      <c r="H22" s="23">
-        <f t="shared" si="1"/>
+      <c r="H22" s="22">
+        <f t="shared" si="2"/>
         <v>1.2292999999999999E-4</v>
       </c>
       <c r="I22" s="2"/>
@@ -3144,21 +3137,21 @@
         <f t="shared" si="0"/>
         <v>12.6</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="19">
         <v>756</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <v>6.81</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="20">
         <v>120.35</v>
       </c>
-      <c r="G23" s="23">
-        <f>E24*0.000001</f>
+      <c r="G23" s="22">
+        <f t="shared" si="1"/>
         <v>3.8399999999999997E-6</v>
       </c>
-      <c r="H23" s="23">
-        <f t="shared" si="1"/>
+      <c r="H23" s="22">
+        <f t="shared" si="2"/>
         <v>1.2034999999999998E-4</v>
       </c>
       <c r="I23" s="2"/>
@@ -3174,21 +3167,21 @@
         <f t="shared" si="0"/>
         <v>13.2</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="19">
         <v>792</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="21">
         <v>3.84</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="20">
         <v>124.12</v>
       </c>
-      <c r="G24" s="23">
-        <f>E25*0.000001</f>
+      <c r="G24" s="22">
+        <f t="shared" si="1"/>
         <v>4.25E-6</v>
       </c>
-      <c r="H24" s="23">
-        <f t="shared" si="1"/>
+      <c r="H24" s="22">
+        <f t="shared" si="2"/>
         <v>1.2412E-4</v>
       </c>
       <c r="I24" s="2"/>
@@ -3204,21 +3197,21 @@
         <f t="shared" si="0"/>
         <v>13.799999999999999</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="19">
         <v>828</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="21">
         <v>4.25</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="20">
         <v>18.2</v>
       </c>
-      <c r="G25" s="23">
-        <f>E26*0.000001</f>
+      <c r="G25" s="22">
+        <f t="shared" si="1"/>
         <v>2.7E-6</v>
       </c>
-      <c r="H25" s="23">
-        <f t="shared" si="1"/>
+      <c r="H25" s="22">
+        <f t="shared" si="2"/>
         <v>1.8199999999999999E-5</v>
       </c>
       <c r="I25" s="2"/>
@@ -3234,21 +3227,21 @@
         <f t="shared" si="0"/>
         <v>14.399999999999999</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="19">
         <v>864</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="21">
         <v>2.7</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="20">
         <v>124.35</v>
       </c>
-      <c r="G26" s="23">
-        <f>E27*0.000001</f>
+      <c r="G26" s="22">
+        <f t="shared" si="1"/>
         <v>2.7599999999999998E-6</v>
       </c>
-      <c r="H26" s="23">
-        <f t="shared" si="1"/>
+      <c r="H26" s="22">
+        <f t="shared" si="2"/>
         <v>1.2434999999999999E-4</v>
       </c>
       <c r="I26" s="2"/>
@@ -3264,21 +3257,21 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="19">
         <v>900</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="21">
         <v>2.76</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="20">
         <v>10.27</v>
       </c>
-      <c r="G27" s="23">
-        <f>E28*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="23">
+      <c r="G27" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="22">
+        <f t="shared" si="2"/>
         <v>1.027E-5</v>
       </c>
       <c r="I27" s="2"/>
@@ -3291,24 +3284,24 @@
         <v>26</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ref="C28:C34" si="2">B28*$K$5</f>
+        <f t="shared" ref="C28:C34" si="3">B28*$K$5</f>
         <v>15.6</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="19">
         <v>936</v>
       </c>
-      <c r="E28" s="22">
-        <v>0</v>
-      </c>
-      <c r="F28" s="21">
+      <c r="E28" s="21">
+        <v>0</v>
+      </c>
+      <c r="F28" s="20">
         <v>55.96</v>
       </c>
-      <c r="G28" s="23">
-        <f>E29*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="23">
+      <c r="G28" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="22">
+        <f t="shared" si="2"/>
         <v>5.596E-5</v>
       </c>
     </row>
@@ -3320,24 +3313,24 @@
         <v>27</v>
       </c>
       <c r="C29" s="1">
+        <f t="shared" si="3"/>
+        <v>16.2</v>
+      </c>
+      <c r="D29" s="19">
+        <v>972</v>
+      </c>
+      <c r="E29" s="21">
+        <v>0</v>
+      </c>
+      <c r="F29" s="20">
+        <v>20.58</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="22">
         <f t="shared" si="2"/>
-        <v>16.2</v>
-      </c>
-      <c r="D29" s="20">
-        <v>972</v>
-      </c>
-      <c r="E29" s="22">
-        <v>0</v>
-      </c>
-      <c r="F29" s="21">
-        <v>20.58</v>
-      </c>
-      <c r="G29" s="23">
-        <f>E30*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="23">
-        <f t="shared" si="1"/>
         <v>2.0579999999999996E-5</v>
       </c>
     </row>
@@ -3349,24 +3342,24 @@
         <v>28</v>
       </c>
       <c r="C30" s="1">
+        <f t="shared" si="3"/>
+        <v>16.8</v>
+      </c>
+      <c r="D30" s="19">
+        <v>1008</v>
+      </c>
+      <c r="E30" s="21">
+        <v>0</v>
+      </c>
+      <c r="F30" s="20">
+        <v>115.78</v>
+      </c>
+      <c r="G30" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="22">
         <f t="shared" si="2"/>
-        <v>16.8</v>
-      </c>
-      <c r="D30" s="20">
-        <v>1008</v>
-      </c>
-      <c r="E30" s="22">
-        <v>0</v>
-      </c>
-      <c r="F30" s="21">
-        <v>115.78</v>
-      </c>
-      <c r="G30" s="23">
-        <f>E31*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="23">
-        <f t="shared" si="1"/>
         <v>1.1577999999999999E-4</v>
       </c>
     </row>
@@ -3378,24 +3371,24 @@
         <v>29</v>
       </c>
       <c r="C31" s="1">
+        <f t="shared" si="3"/>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D31" s="19">
+        <v>1044</v>
+      </c>
+      <c r="E31" s="21">
+        <v>0</v>
+      </c>
+      <c r="F31" s="20">
+        <v>119.98</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="22">
         <f t="shared" si="2"/>
-        <v>17.399999999999999</v>
-      </c>
-      <c r="D31" s="20">
-        <v>1044</v>
-      </c>
-      <c r="E31" s="22">
-        <v>0</v>
-      </c>
-      <c r="F31" s="21">
-        <v>119.98</v>
-      </c>
-      <c r="G31" s="23">
-        <f>E32*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="23">
-        <f t="shared" si="1"/>
         <v>1.1998E-4</v>
       </c>
     </row>
@@ -3407,24 +3400,24 @@
         <v>30</v>
       </c>
       <c r="C32" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="D32" s="19">
+        <v>1080</v>
+      </c>
+      <c r="E32" s="21">
+        <v>0</v>
+      </c>
+      <c r="F32" s="20">
+        <v>33.82</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="22">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="D32" s="20">
-        <v>1080</v>
-      </c>
-      <c r="E32" s="22">
-        <v>0</v>
-      </c>
-      <c r="F32" s="21">
-        <v>33.82</v>
-      </c>
-      <c r="G32" s="23">
-        <f>E33*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="23">
-        <f t="shared" si="1"/>
         <v>3.3819999999999998E-5</v>
       </c>
     </row>
@@ -3436,24 +3429,24 @@
         <v>31</v>
       </c>
       <c r="C33" s="1">
+        <f t="shared" si="3"/>
+        <v>18.599999999999998</v>
+      </c>
+      <c r="D33" s="19">
+        <v>1116</v>
+      </c>
+      <c r="E33" s="21">
+        <v>0</v>
+      </c>
+      <c r="F33" s="20">
+        <v>120.22</v>
+      </c>
+      <c r="G33" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="22">
         <f t="shared" si="2"/>
-        <v>18.599999999999998</v>
-      </c>
-      <c r="D33" s="20">
-        <v>1116</v>
-      </c>
-      <c r="E33" s="22">
-        <v>0</v>
-      </c>
-      <c r="F33" s="21">
-        <v>120.22</v>
-      </c>
-      <c r="G33" s="23">
-        <f>E34*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="23">
-        <f t="shared" si="1"/>
         <v>1.2022E-4</v>
       </c>
     </row>
@@ -3465,24 +3458,24 @@
         <v>32</v>
       </c>
       <c r="C34" s="1">
+        <f t="shared" si="3"/>
+        <v>19.2</v>
+      </c>
+      <c r="D34" s="19">
+        <v>1152</v>
+      </c>
+      <c r="E34" s="21">
+        <v>0</v>
+      </c>
+      <c r="F34" s="20">
+        <v>123.32</v>
+      </c>
+      <c r="G34" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="22">
         <f t="shared" si="2"/>
-        <v>19.2</v>
-      </c>
-      <c r="D34" s="20">
-        <v>1152</v>
-      </c>
-      <c r="E34" s="22">
-        <v>0</v>
-      </c>
-      <c r="F34" s="21">
-        <v>123.32</v>
-      </c>
-      <c r="G34" s="23">
-        <f>E35*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="23">
-        <f t="shared" si="1"/>
         <v>1.2331999999999998E-4</v>
       </c>
     </row>
@@ -3496,38 +3489,36 @@
       <c r="C35" s="3">
         <v>19.8</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="23">
         <v>1188</v>
       </c>
-      <c r="E35" s="29">
-        <v>0</v>
-      </c>
-      <c r="F35" s="29">
+      <c r="E35" s="24">
+        <v>0</v>
+      </c>
+      <c r="F35" s="24">
         <v>5.858E-2</v>
       </c>
-      <c r="G35" s="23">
-        <f>E36*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="23">
+      <c r="G35" s="22">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="22">
+        <f t="shared" si="2"/>
         <v>5.8579999999999999E-8</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C36" s="4"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C37" s="24"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -4289,15 +4280,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010048117A934AEAC441AF47E945F1AED0C0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7272456f5b53c8ae1c345851aef95d27">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c39f1452-4462-4979-941b-c1317cfd14ce" xmlns:ns3="60199b31-2299-4531-8872-a3eaba744cbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16ed4d68a838bfbb08a7468a1792fb8f" ns2:_="" ns3:_="">
     <xsd:import namespace="c39f1452-4462-4979-941b-c1317cfd14ce"/>
@@ -4554,15 +4536,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF42137A-B7F2-4A60-BAD9-4B8683F12BBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4579,4 +4562,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>